<commit_message>
Hoja de Organizacion de Datos v2 (Excel)
</commit_message>
<xml_diff>
--- a/Organizacion de datos Tarea 1 IP.xlsx
+++ b/Organizacion de datos Tarea 1 IP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luciano\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41450002-61C3-4DBC-9DE6-C74AEDBB4F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D815A5-BE9C-4F77-8E29-EEF26D192574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="2550" windowWidth="24240" windowHeight="13140" xr2:uid="{EB6CD720-7883-4599-8674-690887614BF0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Zapato A</t>
   </si>
@@ -125,6 +125,15 @@
   <si>
     <t>Computacion [5]</t>
   </si>
+  <si>
+    <t>Ganancias Estimadas</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>SubTotal:</t>
+  </si>
 </sst>
 </file>
 
@@ -187,11 +196,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBBBB30F-C29F-4ADE-9FB4-7AF6A8335EC8}">
-  <dimension ref="A1:AB100"/>
+  <dimension ref="A1:AB106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,6 +536,7 @@
     <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -545,7 +558,9 @@
       <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -588,7 +603,10 @@
       <c r="F2" s="1">
         <v>6</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1">
+        <f>E2*F2</f>
+        <v>150000</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -617,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C30" si="0">SUM(B3+1)</f>
+        <f t="shared" ref="C3:C34" si="0">SUM(B3+1)</f>
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -629,7 +647,10 @@
       <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1">
+        <f>E3*F3</f>
+        <v>120000</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -670,7 +691,10 @@
       <c r="F4" s="1">
         <v>4</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <f>E4*F4</f>
+        <v>132000</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -711,7 +735,10 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <f>E5*F5</f>
+        <v>144000</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -740,8 +767,13 @@
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1">
+        <f>SUM(G2:G5)</f>
+        <v>546000</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -765,25 +797,12 @@
       <c r="AB6" s="1"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F7" s="1">
-        <v>10</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -808,24 +827,29 @@
       <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="1">
-        <v>15000</v>
+        <v>12000</v>
       </c>
       <c r="F8" s="1">
         <v>10</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <f>E8*F8</f>
+        <v>120000</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -851,22 +875,25 @@
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1">
-        <v>7000</v>
+        <v>15000</v>
       </c>
       <c r="F9" s="1">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
+        <f>E9*F9</f>
+        <v>150000</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -892,22 +919,25 @@
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="1">
-        <v>12000</v>
+        <v>7000</v>
       </c>
       <c r="F10" s="1">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="1">
+        <f>E10*F10</f>
+        <v>56000</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -933,22 +963,25 @@
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1">
-        <v>20000</v>
+        <v>12000</v>
       </c>
       <c r="F11" s="1">
-        <v>5</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G11" s="1">
+        <f>E11*F11</f>
+        <v>120000</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -974,22 +1007,25 @@
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1">
-        <v>21000</v>
+        <v>20000</v>
       </c>
       <c r="F12" s="1">
-        <v>6</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="1">
+        <f>E12*F12</f>
+        <v>100000</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1014,12 +1050,26 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="B13" s="2">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1">
+        <v>21000</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1">
+        <f>E13*F13</f>
+        <v>126000</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1043,26 +1093,18 @@
       <c r="AB13" s="1"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="1">
-        <v>15000</v>
-      </c>
-      <c r="F14" s="1">
-        <v>5</v>
-      </c>
-      <c r="G14" s="1"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="1">
+        <f>SUM(G8:G13)</f>
+        <v>672000</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1087,22 +1129,11 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1">
-        <v>20000</v>
-      </c>
-      <c r="F15" s="1">
-        <v>5</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1127,24 +1158,29 @@
       <c r="AB15" s="1"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B16" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="F16" s="1">
-        <v>10</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G3:G34" si="1">E16*F16</f>
+        <v>75000</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1170,22 +1206,25 @@
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1">
-        <v>12000</v>
+        <v>20000</v>
       </c>
       <c r="F17" s="1">
-        <v>10</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1211,22 +1250,25 @@
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E18" s="1">
-        <v>18000</v>
+        <v>10000</v>
       </c>
       <c r="F18" s="1">
-        <v>6</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1252,22 +1294,25 @@
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1">
-        <v>20000</v>
+        <v>12000</v>
       </c>
       <c r="F19" s="1">
-        <v>6</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1292,12 +1337,26 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="B20" s="2">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1">
+        <v>18000</v>
+      </c>
+      <c r="F20" s="1">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>108000</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1321,26 +1380,27 @@
       <c r="AB20" s="1"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A21" s="1"/>
       <c r="B21" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1365,23 +1425,17 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="1">
-        <v>55000</v>
-      </c>
-      <c r="F22" s="1">
-        <v>3</v>
-      </c>
-      <c r="G22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="1">
+        <f>SUM(G16:G21)</f>
+        <v>623000</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1406,22 +1460,11 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2">
-        <v>2</v>
-      </c>
-      <c r="C23" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="1">
-        <v>200000</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1446,24 +1489,29 @@
       <c r="AB23" s="1"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B24" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E24" s="1">
-        <v>350000</v>
+        <v>50000</v>
       </c>
       <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1489,22 +1537,25 @@
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E25" s="1">
-        <v>250000</v>
+        <v>55000</v>
       </c>
       <c r="F25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="1"/>
+        <v>165000</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1529,12 +1580,26 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1">
+        <v>200000</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="1"/>
+        <v>200000</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1558,26 +1623,27 @@
       <c r="AB26" s="1"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A27" s="1"/>
       <c r="B27" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E27" s="1">
-        <v>500000</v>
+        <v>350000</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1">
+        <f t="shared" si="1"/>
+        <v>350000</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1603,22 +1669,25 @@
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E28" s="1">
-        <v>800000</v>
+        <v>250000</v>
       </c>
       <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="1"/>
+        <v>250000</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1643,23 +1712,17 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="2">
-        <v>2</v>
-      </c>
-      <c r="C29" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="1">
-        <v>220000</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="1">
+        <f>SUM(G24:G28)</f>
+        <v>1065000</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1684,22 +1747,11 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="2">
-        <v>3</v>
-      </c>
-      <c r="C30" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="1">
-        <v>999990</v>
-      </c>
-      <c r="F30" s="1">
-        <v>2</v>
-      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1724,13 +1776,29 @@
       <c r="AB30" s="1"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="1">
+        <v>500000</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="1"/>
+        <v>500000</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1755,12 +1823,26 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="1">
+        <v>800000</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="1"/>
+        <v>1600000</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1785,12 +1867,26 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="B33" s="2">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="1">
+        <v>220000</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="1"/>
+        <v>220000</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1815,12 +1911,26 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="B34" s="2">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="1">
+        <v>999990</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="1"/>
+        <v>1999980</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1845,12 +1955,17 @@
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="F35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="1">
+        <f>SUM(G31:G34)</f>
+        <v>4319980</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1875,11 +1990,11 @@
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="F36" s="3"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -1909,8 +2024,13 @@
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="F37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="1">
+        <f>SUM(G35,G29,G22,G14,G6)</f>
+        <v>7225980</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -3823,6 +3943,186 @@
       <c r="AA100" s="1"/>
       <c r="AB100" s="1"/>
     </row>
+    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
+      <c r="Z101" s="1"/>
+      <c r="AA101" s="1"/>
+      <c r="AB101" s="1"/>
+    </row>
+    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
+      <c r="T102" s="1"/>
+      <c r="U102" s="1"/>
+      <c r="V102" s="1"/>
+      <c r="W102" s="1"/>
+      <c r="X102" s="1"/>
+      <c r="Y102" s="1"/>
+      <c r="Z102" s="1"/>
+      <c r="AA102" s="1"/>
+      <c r="AB102" s="1"/>
+    </row>
+    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="1"/>
+      <c r="S103" s="1"/>
+      <c r="T103" s="1"/>
+      <c r="U103" s="1"/>
+      <c r="V103" s="1"/>
+      <c r="W103" s="1"/>
+      <c r="X103" s="1"/>
+      <c r="Y103" s="1"/>
+      <c r="Z103" s="1"/>
+      <c r="AA103" s="1"/>
+      <c r="AB103" s="1"/>
+    </row>
+    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="1"/>
+      <c r="S104" s="1"/>
+      <c r="T104" s="1"/>
+      <c r="U104" s="1"/>
+      <c r="V104" s="1"/>
+      <c r="W104" s="1"/>
+      <c r="X104" s="1"/>
+      <c r="Y104" s="1"/>
+      <c r="Z104" s="1"/>
+      <c r="AA104" s="1"/>
+      <c r="AB104" s="1"/>
+    </row>
+    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="1"/>
+      <c r="S105" s="1"/>
+      <c r="T105" s="1"/>
+      <c r="U105" s="1"/>
+      <c r="V105" s="1"/>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+      <c r="Y105" s="1"/>
+      <c r="Z105" s="1"/>
+      <c r="AA105" s="1"/>
+      <c r="AB105" s="1"/>
+    </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+      <c r="R106" s="1"/>
+      <c r="S106" s="1"/>
+      <c r="T106" s="1"/>
+      <c r="U106" s="1"/>
+      <c r="V106" s="1"/>
+      <c r="W106" s="1"/>
+      <c r="X106" s="1"/>
+      <c r="Y106" s="1"/>
+      <c r="Z106" s="1"/>
+      <c r="AA106" s="1"/>
+      <c r="AB106" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>